<commit_message>
Fixed movement with dialogue
</commit_message>
<xml_diff>
--- a/Копия Dialogues.xlsx
+++ b/Копия Dialogues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plesk\Desktop\super_game\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\makst\Desktop\WorkSpace\Games_Unity\super_game\Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C954C81F-1FEC-4176-BCFE-BBBC4255E9C2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD4BCF5-3379-4C45-9C3B-07D6C5BCC8DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dialogues" sheetId="1" r:id="rId1"/>
@@ -900,12 +900,15 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -913,7 +916,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>

</xml_diff>